<commit_message>
update part 3: adjust get_alpha() to monthly return
</commit_message>
<xml_diff>
--- a/output/part3/5. ew_sheet.xlsx
+++ b/output/part3/5. ew_sheet.xlsx
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.02525151711060743</v>
+        <v>0.007715731536047051</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.07217374818243145</v>
+        <v>0.01072926463919976</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.13595584697328</v>
+        <v>0.01313059040095384</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.2704860572557466</v>
+        <v>0.01533374246478889</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-3.141540881407813</v>
+        <v>2.960985194873507</v>
       </c>
       <c r="C3" t="n">
-        <v>-5.659212437873948</v>
+        <v>5.278654477475951</v>
       </c>
       <c r="D3" t="n">
-        <v>-8.178921413281191</v>
+        <v>7.920378794277832</v>
       </c>
       <c r="E3" t="n">
-        <v>-5.149773834672087</v>
+        <v>6.154797652350622</v>
       </c>
     </row>
     <row r="4">
@@ -500,17 +500,15 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.05456776632690262</v>
+        <v>-0.01923241907602552</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1164341818590278</v>
+        <v>-0.02211886608468998</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1767539485893067</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.2369722645730672</v>
-      </c>
+        <v>-0.02496364126227692</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -519,17 +517,15 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7.226340550630453</v>
+        <v>-7.248605109103126</v>
       </c>
       <c r="C5" t="n">
-        <v>8.524197123913291</v>
+        <v>-8.497494301771022</v>
       </c>
       <c r="D5" t="n">
-        <v>8.640719782127375</v>
-      </c>
-      <c r="E5" t="n">
-        <v>8.209690843748909</v>
-      </c>
+        <v>-8.279145604947555</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -538,17 +534,15 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.02931624921629521</v>
+        <v>0.008306192841956505</v>
       </c>
       <c r="C6" t="n">
-        <v>0.04426043367659634</v>
+        <v>0.004700624964746629</v>
       </c>
       <c r="D6" t="n">
-        <v>0.04079810161602659</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-0.03351379268267938</v>
-      </c>
+        <v>0.0008618560449260675</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -557,17 +551,15 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.599289274123679</v>
+        <v>2.19958781331111</v>
       </c>
       <c r="C7" t="n">
-        <v>2.319655325483023</v>
+        <v>1.449288110650679</v>
       </c>
       <c r="D7" t="n">
-        <v>1.570184440997291</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-0.5811419000487997</v>
-      </c>
+        <v>0.2842886919970967</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -576,16 +568,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.02692998592764881</v>
+        <v>0.008357527046492438</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.0795540492949111</v>
+        <v>0.01192195670660364</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1528732139853863</v>
+        <v>0.01434129409155893</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.2908742632860035</v>
+        <v>0.01681369197704382</v>
       </c>
     </row>
     <row r="9">
@@ -595,16 +587,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-3.569825016394807</v>
+        <v>3.423039717211485</v>
       </c>
       <c r="C9" t="n">
-        <v>-6.299270576669085</v>
+        <v>5.899705947516384</v>
       </c>
       <c r="D9" t="n">
-        <v>-5.236100190425912</v>
+        <v>6.631425257262459</v>
       </c>
       <c r="E9" t="n">
-        <v>-5.35587910756238</v>
+        <v>6.430676064501979</v>
       </c>
     </row>
     <row r="10">
@@ -614,17 +606,15 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.05376934432887132</v>
+        <v>-0.01895423313014715</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1065743726732037</v>
+        <v>-0.02017157522180509</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1695114004897026</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.2216549495190103</v>
-      </c>
+        <v>-0.02473949831779778</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -633,17 +623,15 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6.936046628690412</v>
+        <v>-6.9755409058152</v>
       </c>
       <c r="C11" t="n">
-        <v>7.884049394480377</v>
+        <v>-7.944255618650784</v>
       </c>
       <c r="D11" t="n">
-        <v>7.921382610109761</v>
-      </c>
-      <c r="E11" t="n">
-        <v>7.51334134234613</v>
-      </c>
+        <v>-7.219447958733066</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -652,17 +640,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.02683935840122249</v>
+        <v>0.007791251779627479</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02702032337829263</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.01663818650431636</v>
-      </c>
-      <c r="E12" t="n">
-        <v>-0.06921931376699318</v>
-      </c>
+        <v>0.00225479725540151</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -671,17 +655,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2.600286238053411</v>
+        <v>2.263420962238378</v>
       </c>
       <c r="C13" t="n">
-        <v>1.48950067444305</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.4662022095171604</v>
-      </c>
-      <c r="E13" t="n">
-        <v>-1.109989436155471</v>
-      </c>
+        <v>0.7330567005423656</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -690,16 +670,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.02925570199445319</v>
+        <v>0.009041690451927127</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.08495076651729522</v>
+        <v>0.01263615281712632</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.1779196846719234</v>
+        <v>0.01594696925871424</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.3137181945316526</v>
+        <v>0.01836798765851275</v>
       </c>
     </row>
     <row r="15">
@@ -709,16 +689,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-3.674461593503881</v>
+        <v>3.479376881707805</v>
       </c>
       <c r="C15" t="n">
-        <v>-6.257255686567006</v>
+        <v>5.834334341290351</v>
       </c>
       <c r="D15" t="n">
-        <v>-5.337483779664187</v>
+        <v>6.492683760118034</v>
       </c>
       <c r="E15" t="n">
-        <v>-6.176895541258522</v>
+        <v>7.104735858558067</v>
       </c>
     </row>
     <row r="16">
@@ -728,17 +708,15 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.04211621706028183</v>
+        <v>-0.01489975316747699</v>
       </c>
       <c r="C16" t="n">
-        <v>0.09104716893734913</v>
+        <v>-0.0174307244100564</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1379704442564882</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.1828269732478789</v>
-      </c>
+        <v>-0.02030460099731261</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -747,17 +725,15 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>5.424954954104059</v>
+        <v>-5.535363787294505</v>
       </c>
       <c r="C17" t="n">
-        <v>6.404058615130687</v>
+        <v>-6.53827035388502</v>
       </c>
       <c r="D17" t="n">
-        <v>6.420448773035746</v>
-      </c>
-      <c r="E17" t="n">
-        <v>6.117987581419295</v>
-      </c>
+        <v>-6.086614299188402</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -766,17 +742,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.01286051506582864</v>
+        <v>0.003228875245632952</v>
       </c>
       <c r="C18" t="n">
-        <v>0.006096402420053919</v>
-      </c>
-      <c r="D18" t="n">
-        <v>-0.0399492404154353</v>
-      </c>
-      <c r="E18" t="n">
-        <v>-0.1308912212837737</v>
-      </c>
+        <v>-0.001599139166869575</v>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -785,17 +757,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.251997737826061</v>
+        <v>0.9402343593677677</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3101435868590505</v>
-      </c>
-      <c r="D19" t="n">
-        <v>-0.9792433031192233</v>
-      </c>
-      <c r="E19" t="n">
-        <v>-2.1732628560856</v>
-      </c>
+        <v>-0.4787012132139899</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -804,16 +772,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.0385976833107571</v>
+        <v>0.01206491642932434</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.1075986279441178</v>
+        <v>0.01610843657722701</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.2195485566391227</v>
+        <v>0.01945519334682248</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.3528007857730613</v>
+        <v>0.02070905493725941</v>
       </c>
     </row>
     <row r="21">
@@ -823,16 +791,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-4.747050121813824</v>
+        <v>4.534244893993776</v>
       </c>
       <c r="C21" t="n">
-        <v>-7.725837968876433</v>
+        <v>7.321129523134057</v>
       </c>
       <c r="D21" t="n">
-        <v>-6.323295268217559</v>
+        <v>7.606929816504106</v>
       </c>
       <c r="E21" t="n">
-        <v>-6.614091404257723</v>
+        <v>7.922102879841858</v>
       </c>
     </row>
     <row r="22">
@@ -842,17 +810,15 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.03997263444418234</v>
+        <v>-0.01426144422137027</v>
       </c>
       <c r="C22" t="n">
-        <v>0.08134785920512219</v>
+        <v>-0.01575796625718798</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1206085172267554</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.1607705001686635</v>
-      </c>
+        <v>-0.01791234271276543</v>
+      </c>
+      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -861,17 +827,15 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4.897346920192891</v>
+        <v>-5.027115627469286</v>
       </c>
       <c r="C23" t="n">
-        <v>5.607052826026679</v>
+        <v>-5.801771728919297</v>
       </c>
       <c r="D23" t="n">
-        <v>5.704552780734814</v>
-      </c>
-      <c r="E23" t="n">
-        <v>5.438063218616265</v>
-      </c>
+        <v>-5.505493227295577</v>
+      </c>
+      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -880,17 +844,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.001374951133425231</v>
+        <v>-0.0007985145805884673</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.02625076873899562</v>
-      </c>
-      <c r="D24" t="n">
-        <v>-0.09894003941236723</v>
-      </c>
-      <c r="E24" t="n">
-        <v>-0.1920302856043978</v>
-      </c>
+        <v>-0.007556686967392715</v>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -899,17 +859,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.1233307169546</v>
+        <v>-0.2135405384522041</v>
       </c>
       <c r="C25" t="n">
-        <v>-1.263388095826291</v>
-      </c>
-      <c r="D25" t="n">
-        <v>-2.320510702518378</v>
-      </c>
-      <c r="E25" t="n">
-        <v>-3.166761817168089</v>
-      </c>
+        <v>-2.094864827514199</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update part 3: adjust get_alpha() to take negative monthly return into consideration
</commit_message>
<xml_diff>
--- a/output/part3/5. ew_sheet.xlsx
+++ b/output/part3/5. ew_sheet.xlsx
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.007715731536047051</v>
+        <v>0.01730024852427183</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01072926463919976</v>
+        <v>0.01743797812681002</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01313059040095384</v>
+        <v>0.01664993251499259</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01533374246478889</v>
+        <v>0.01580140637326485</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.960985194873507</v>
+        <v>7.164600579590038</v>
       </c>
       <c r="C3" t="n">
-        <v>5.278654477475951</v>
+        <v>8.34981664908516</v>
       </c>
       <c r="D3" t="n">
-        <v>7.920378794277832</v>
+        <v>8.466001735709472</v>
       </c>
       <c r="E3" t="n">
-        <v>6.154797652350622</v>
+        <v>8.287056293015256</v>
       </c>
     </row>
     <row r="4">
@@ -500,15 +500,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.01923241907602552</v>
+        <v>-0.007715731536047051</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.02211886608468998</v>
+        <v>-0.01072926463919976</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.02496364126227692</v>
-      </c>
-      <c r="E4" t="inlineStr"/>
+        <v>-0.01313059040095384</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.01533374246478889</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -517,15 +519,17 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-7.248605109103126</v>
+        <v>-2.960985194873507</v>
       </c>
       <c r="C5" t="n">
-        <v>-8.497494301771022</v>
+        <v>-5.278654477475951</v>
       </c>
       <c r="D5" t="n">
-        <v>-8.279145604947555</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
+        <v>-7.920378794277832</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-6.154797652350622</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -534,15 +538,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.008306192841956505</v>
+        <v>0.001939250719171284</v>
       </c>
       <c r="C6" t="n">
-        <v>0.004700624964746629</v>
+        <v>0.002214536068434529</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0008618560449260675</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
+        <v>0.0005560889073582502</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.00124476984616817</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -551,15 +557,17 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.19958781331111</v>
+        <v>2.043383266899122</v>
       </c>
       <c r="C7" t="n">
-        <v>1.449288110650679</v>
+        <v>1.35957417776543</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2842886919970967</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+        <v>0.2438515610454587</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-0.4164969276094324</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -568,16 +576,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.008357527046492438</v>
+        <v>0.01704408369759636</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01192195670660364</v>
+        <v>0.01599109251986152</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01434129409155893</v>
+        <v>0.01592105532579664</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01681369197704382</v>
+        <v>0.0147756170397372</v>
       </c>
     </row>
     <row r="9">
@@ -587,16 +595,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3.423039717211485</v>
+        <v>6.859552101866575</v>
       </c>
       <c r="C9" t="n">
-        <v>5.899705947516384</v>
+        <v>7.691104751428291</v>
       </c>
       <c r="D9" t="n">
-        <v>6.631425257262459</v>
+        <v>7.928774249915929</v>
       </c>
       <c r="E9" t="n">
-        <v>6.430676064501979</v>
+        <v>7.699502759219947</v>
       </c>
     </row>
     <row r="10">
@@ -606,15 +614,17 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.01895423313014715</v>
+        <v>-0.008357527046492438</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.02017157522180509</v>
+        <v>-0.01192195670660364</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.02473949831779778</v>
-      </c>
-      <c r="E10" t="inlineStr"/>
+        <v>-0.01434129409155893</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-0.01681369197704382</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -623,15 +633,17 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-6.9755409058152</v>
+        <v>-3.423039717211485</v>
       </c>
       <c r="C11" t="n">
-        <v>-7.944255618650784</v>
+        <v>-5.899705947516384</v>
       </c>
       <c r="D11" t="n">
-        <v>-7.219447958733066</v>
-      </c>
-      <c r="E11" t="inlineStr"/>
+        <v>-6.631425257262459</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-6.430676064501979</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -640,13 +652,17 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.007791251779627479</v>
+        <v>0.001840024300327477</v>
       </c>
       <c r="C12" t="n">
-        <v>0.00225479725540151</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+        <v>0.001011729802501773</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.0007448541283637865</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.003541466442669543</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -655,13 +671,17 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2.263420962238378</v>
+        <v>2.132812360357899</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7330567005423656</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+        <v>0.6551861297420783</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.3266746206261197</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-1.133678317260042</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -670,16 +690,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.009041690451927127</v>
+        <v>0.01328894048839277</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01263615281712632</v>
+        <v>0.01352169674337987</v>
       </c>
       <c r="D14" t="n">
-        <v>0.01594696925871424</v>
+        <v>0.01281321607820902</v>
       </c>
       <c r="E14" t="n">
-        <v>0.01836798765851275</v>
+        <v>0.01202016398799491</v>
       </c>
     </row>
     <row r="15">
@@ -689,16 +709,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3.479376881707805</v>
+        <v>5.291025205464209</v>
       </c>
       <c r="C15" t="n">
-        <v>5.834334341290351</v>
+        <v>6.178792138611436</v>
       </c>
       <c r="D15" t="n">
-        <v>6.492683760118034</v>
+        <v>6.269227790973541</v>
       </c>
       <c r="E15" t="n">
-        <v>7.104735858558067</v>
+        <v>6.213169556932412</v>
       </c>
     </row>
     <row r="16">
@@ -708,15 +728,17 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.01489975316747699</v>
+        <v>-0.009041690451927127</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.0174307244100564</v>
+        <v>-0.01263615281712632</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.02030460099731261</v>
-      </c>
-      <c r="E16" t="inlineStr"/>
+        <v>-0.01594696925871424</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.01836798765851275</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -725,15 +747,17 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-5.535363787294505</v>
+        <v>-3.479376881707805</v>
       </c>
       <c r="C17" t="n">
-        <v>-6.53827035388502</v>
+        <v>-5.834334341290351</v>
       </c>
       <c r="D17" t="n">
-        <v>-6.086614299188402</v>
-      </c>
-      <c r="E17" t="inlineStr"/>
+        <v>-6.492683760118034</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-7.104735858558067</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -742,13 +766,17 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.003228875245632952</v>
+        <v>0.0007076709781948513</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.001599139166869575</v>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+        <v>-0.0009347170612388165</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.003639369204604907</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.007236591819227384</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -757,13 +785,17 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.9402343593677677</v>
+        <v>0.8218775133873167</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.4787012132139899</v>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+        <v>-0.5576268074890148</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-1.520988649219853</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-2.207458316196834</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -772,16 +804,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.01206491642932434</v>
+        <v>0.01250928047880678</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01610843657722701</v>
+        <v>0.01195200433994183</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01945519334682248</v>
+        <v>0.01111592538759691</v>
       </c>
       <c r="E20" t="n">
-        <v>0.02070905493725941</v>
+        <v>0.01046191925249658</v>
       </c>
     </row>
     <row r="21">
@@ -791,16 +823,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4.534244893993776</v>
+        <v>4.743679683272769</v>
       </c>
       <c r="C21" t="n">
-        <v>7.321129523134057</v>
+        <v>5.346723612849027</v>
       </c>
       <c r="D21" t="n">
-        <v>7.606929816504106</v>
+        <v>5.535115477684325</v>
       </c>
       <c r="E21" t="n">
-        <v>7.922102879841858</v>
+        <v>5.442017002352673</v>
       </c>
     </row>
     <row r="22">
@@ -810,15 +842,17 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.01426144422137027</v>
+        <v>-0.01206491642932434</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.01575796625718798</v>
+        <v>-0.01610843657722701</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.01791234271276543</v>
-      </c>
-      <c r="E22" t="inlineStr"/>
+        <v>-0.01945519334682248</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-0.02070905493725941</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -827,15 +861,17 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-5.027115627469286</v>
+        <v>-4.534244893993776</v>
       </c>
       <c r="C23" t="n">
-        <v>-5.801771728919297</v>
+        <v>-7.321129523134057</v>
       </c>
       <c r="D23" t="n">
-        <v>-5.505493227295577</v>
-      </c>
-      <c r="E23" t="inlineStr"/>
+        <v>-7.606929816504106</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-7.922102879841858</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -844,13 +880,17 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.0007985145805884673</v>
+        <v>-0.0003187444768624916</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.007556686967392715</v>
-      </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+        <v>-0.003946282955426309</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-0.006035399194845385</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-0.008727206880805066</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -859,13 +899,17 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.2135405384522041</v>
+        <v>-0.3395441319129954</v>
       </c>
       <c r="C25" t="n">
-        <v>-2.094864827514199</v>
-      </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
+        <v>-2.174803074233515</v>
+      </c>
+      <c r="D25" t="n">
+        <v>-2.464360799951158</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-2.230996129500106</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>